<commit_message>
Aggiornati limiti richieste risorse k8s
</commit_message>
<xml_diff>
--- a/docs/Resource request kubernetes.xlsx
+++ b/docs/Resource request kubernetes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fausto/Developer/Progetti/Unimib/bigtwine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D415D1-539B-744C-A298-3D751018E008}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B81F0DB-D6A5-7548-A4F4-8CF0A72C1366}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{88325B8C-A9E7-804C-9430-2AFBA498DB59}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -140,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +459,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C5" s="1">
         <v>0.5</v>
@@ -588,10 +588,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="2">
         <v>256</v>
@@ -611,10 +611,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C7" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="2">
         <v>256</v>
@@ -847,11 +847,11 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <f>SUM(B2:B16)</f>
-        <v>3.2500000000000009</v>
+        <v>3.5500000000000007</v>
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C16)</f>
-        <v>10.4</v>
+        <v>10.9</v>
       </c>
       <c r="D18" s="1">
         <f>SUM(D2:D16)</f>

</xml_diff>